<commit_message>
Añadiendo listar comentario y listar usuarios
</commit_message>
<xml_diff>
--- a/Pasos.xlsx
+++ b/Pasos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="18915" windowHeight="6720"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18915" windowHeight="6720" tabRatio="384"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Pasos para la web por parte de un usuario</t>
   </si>
@@ -166,6 +166,15 @@
   </si>
   <si>
     <t>Método (GET)</t>
+  </si>
+  <si>
+    <t>10 - Listar usuarios</t>
+  </si>
+  <si>
+    <t>app.get(urls.users,isUser, listUsers)</t>
+  </si>
+  <si>
+    <t>sólo me sale para un campo</t>
   </si>
 </sst>
 </file>
@@ -707,10 +716,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D8:J20"/>
+  <dimension ref="D8:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E3" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +938,30 @@
       <c r="H20" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="I20" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="J20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D21" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="J21" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Voto sercio comprobado y funcion modificarDatos
</commit_message>
<xml_diff>
--- a/Pasos.xlsx
+++ b/Pasos.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Pasos para la web por parte de un usuario</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>sólo me sale para un campo</t>
+  </si>
+  <si>
+    <t>app.post("/servicios/votar/:id_servicio/:id_solucionador",isUser, voteServicio);</t>
+  </si>
+  <si>
+    <t>Método (POST)</t>
+  </si>
+  <si>
+    <t>11 - Puntuar</t>
   </si>
 </sst>
 </file>
@@ -359,7 +368,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -414,6 +423,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -716,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D8:J21"/>
+  <dimension ref="D8:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E6" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -728,7 +740,7 @@
     <col min="4" max="4" width="38.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17" style="1" customWidth="1"/>
     <col min="6" max="6" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="67.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="75.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="18.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="42.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="11.42578125" style="1"/>
@@ -962,6 +974,23 @@
         <v>38</v>
       </c>
       <c r="J21" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="D22" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="27" t="s">
+        <v>39</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J22" s="1" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Primera conexión con el back, devuelve token
</commit_message>
<xml_diff>
--- a/Pasos.xlsx
+++ b/Pasos.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="150" windowWidth="18915" windowHeight="6720" tabRatio="480" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="150" windowWidth="18915" windowHeight="6720" tabRatio="480" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="4" r:id="rId1"/>
     <sheet name="End-points" sheetId="5" r:id="rId2"/>
+    <sheet name="Relación con Front - RUTAS URL" sheetId="6" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'End-points'!$E$5:$M$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$C$8:$O$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'End-points'!$E$5:$M$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Resumen!$C$8:$O$24</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="139">
   <si>
     <t>End-point</t>
   </si>
@@ -655,12 +656,48 @@
   <si>
     <t>Obxeto Url</t>
   </si>
+  <si>
+    <t>Petición</t>
+  </si>
+  <si>
+    <t>Con Postman</t>
+  </si>
+  <si>
+    <t>Desde React</t>
+  </si>
+  <si>
+    <t>servicios/borrar/113</t>
+  </si>
+  <si>
+    <t>servicios/borrar/${id_ser}</t>
+  </si>
+  <si>
+    <t>/users/delete/{id}</t>
+  </si>
+  <si>
+    <t>la dá el correo</t>
+  </si>
+  <si>
+    <t>/users/delete/comentario/{id}</t>
+  </si>
+  <si>
+    <t>/users/edit/{id}</t>
+  </si>
+  <si>
+    <t>/users/insert/comentario</t>
+  </si>
+  <si>
+    <t>/servicios/votar/{id_servicio}/{id_solucionador}</t>
+  </si>
+  <si>
+    <t>/users/userLogin</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -777,6 +814,14 @@
     <font>
       <b/>
       <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -958,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1082,6 +1127,36 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1090,33 +1165,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1126,6 +1174,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF4BEB35"/>
       <color rgb="FFAED816"/>
     </mruColors>
   </colors>
@@ -1426,8 +1475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A6:P44"/>
   <sheetViews>
-    <sheetView topLeftCell="D4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView topLeftCell="F4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,11 +1499,11 @@
     </row>
     <row r="7" spans="1:16" ht="18.75" x14ac:dyDescent="0.3">
       <c r="F7" s="2"/>
-      <c r="G7" s="62" t="s">
+      <c r="G7" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="62"/>
-      <c r="I7" s="62"/>
+      <c r="H7" s="60"/>
+      <c r="I7" s="60"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
       <c r="L7" s="9"/>
@@ -1494,7 +1543,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C9" s="59" t="s">
+      <c r="C9" s="57" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3"/>
@@ -1526,7 +1575,7 @@
       <c r="P9" s="1"/>
     </row>
     <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C10" s="59"/>
+      <c r="C10" s="57"/>
       <c r="D10" s="3"/>
       <c r="E10" s="8" t="s">
         <v>47</v>
@@ -1556,7 +1605,7 @@
       <c r="P10" s="1"/>
     </row>
     <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="C11" s="59"/>
+      <c r="C11" s="57"/>
       <c r="D11" s="3" t="s">
         <v>63</v>
       </c>
@@ -1589,7 +1638,7 @@
     </row>
     <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C12" s="20"/>
-      <c r="D12" s="58" t="s">
+      <c r="D12" s="56" t="s">
         <v>64</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -1622,7 +1671,7 @@
       <c r="C13" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="58"/>
+      <c r="D13" s="56"/>
       <c r="E13" s="4" t="s">
         <v>13</v>
       </c>
@@ -1656,7 +1705,7 @@
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="22"/>
-      <c r="D14" s="58"/>
+      <c r="D14" s="56"/>
       <c r="E14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1686,10 +1735,10 @@
     <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
-      <c r="C15" s="60" t="s">
+      <c r="C15" s="58" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="58" t="s">
+      <c r="D15" s="56" t="s">
         <v>64</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -1721,8 +1770,8 @@
     <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="56"/>
       <c r="E16" s="4" t="s">
         <v>17</v>
       </c>
@@ -1752,10 +1801,10 @@
     <row r="17" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
-      <c r="C17" s="51" t="s">
+      <c r="C17" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="52" t="s">
+      <c r="D17" s="62" t="s">
         <v>64</v>
       </c>
       <c r="E17" s="12" t="s">
@@ -1787,8 +1836,8 @@
     <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="53"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="63"/>
       <c r="E18" s="12" t="s">
         <v>14</v>
       </c>
@@ -1882,7 +1931,7 @@
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="52" t="s">
         <v>41</v>
       </c>
       <c r="D21" s="12" t="s">
@@ -1915,7 +1964,7 @@
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C22" s="55"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="4" t="s">
         <v>64</v>
       </c>
@@ -1946,7 +1995,7 @@
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C23" s="56"/>
+      <c r="C23" s="54"/>
       <c r="D23" s="4" t="s">
         <v>64</v>
       </c>
@@ -2008,14 +2057,14 @@
       </c>
     </row>
     <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="G26" s="57"/>
-      <c r="H26" s="57"/>
-      <c r="I26" s="57"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="57"/>
-      <c r="M26" s="57"/>
-      <c r="N26" s="57"/>
+      <c r="G26" s="55"/>
+      <c r="H26" s="55"/>
+      <c r="I26" s="55"/>
+      <c r="J26" s="55"/>
+      <c r="K26" s="55"/>
+      <c r="L26" s="55"/>
+      <c r="M26" s="55"/>
+      <c r="N26" s="55"/>
     </row>
     <row r="27" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J27" s="11"/>
@@ -2079,17 +2128,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C8:O20"/>
+  <autoFilter ref="C8:O24"/>
   <mergeCells count="9">
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D12:D14"/>
     <mergeCell ref="G7:I7"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="C21:C23"/>
     <mergeCell ref="G26:N26"/>
     <mergeCell ref="D15:D16"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D12:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2101,14 +2150,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="E5:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="107.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.140625" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="23.85546875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="46.7109375" bestFit="1" customWidth="1"/>
@@ -2586,7 +2635,254 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E5:M5"/>
+  <autoFilter ref="E5:M21"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E5:H21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="97.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="42.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E5" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="G5" t="s">
+        <v>128</v>
+      </c>
+      <c r="H5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="6" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E6" t="str">
+        <f>'End-points'!E6</f>
+        <v>app.post(urls.insertUser,newUser)</v>
+      </c>
+      <c r="F6" t="str">
+        <f>'End-points'!I6</f>
+        <v>/users/insertar</v>
+      </c>
+      <c r="H6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E7" t="str">
+        <f>'End-points'!E7</f>
+        <v>app.get(urls.validaregistrationCode,validateUser)</v>
+      </c>
+      <c r="F7" t="str">
+        <f>'End-points'!I7</f>
+        <v>/validar/:registrationCode</v>
+      </c>
+      <c r="H7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E8" t="str">
+        <f>'End-points'!E8</f>
+        <v xml:space="preserve">app.post(urlsusers.userslogin, loginUser);   </v>
+      </c>
+      <c r="F8" t="str">
+        <f>'End-points'!I8</f>
+        <v>/users/login</v>
+      </c>
+      <c r="H8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="9" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E9" t="str">
+        <f>'End-points'!E9</f>
+        <v>app.delete(urlsusers.deleteuser,isUser,userExists,canDeleteUser, deleteUser)</v>
+      </c>
+      <c r="F9" t="str">
+        <f>'End-points'!I9</f>
+        <v>/users/delete/:id</v>
+      </c>
+      <c r="H9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E10" t="str">
+        <f>'End-points'!E10</f>
+        <v>app.delete(urls.deleteservicio, isUser, servicioExist, canDeleteService,deleteServicio)</v>
+      </c>
+      <c r="F10" t="str">
+        <f>'End-points'!I10</f>
+        <v>/servicios/borrar/:id_ser</v>
+      </c>
+      <c r="G10" t="s">
+        <v>130</v>
+      </c>
+      <c r="H10" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E11" t="str">
+        <f>'End-points'!E11</f>
+        <v xml:space="preserve">app.delete(urlsusers.userborracomentario, isUser,comentarioExists,canDeleteComentar,deleteComentar) </v>
+      </c>
+      <c r="F11" t="str">
+        <f>'End-points'!I11</f>
+        <v>/users/delete/comentario/:id</v>
+      </c>
+      <c r="H11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="12" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E12" t="str">
+        <f>'End-points'!E12</f>
+        <v>app.put(urlsusers.updateuser,isUser,userExists, canEdit ,editUser)</v>
+      </c>
+      <c r="F12" t="str">
+        <f>'End-points'!I12</f>
+        <v>/users/edit/:id</v>
+      </c>
+      <c r="H12" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E13" t="str">
+        <f>'End-points'!E13</f>
+        <v>app.post(urls.admin,isUser,userExists,canEditAmin,updateAmin)</v>
+      </c>
+      <c r="F13" t="str">
+        <f>'End-points'!I13</f>
+        <v>/admin/modificar/</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E14" t="str">
+        <f>'End-points'!E14</f>
+        <v>app.post(urls.servicios, isUser,canInsertService,newServicio)</v>
+      </c>
+      <c r="F14" t="str">
+        <f>'End-points'!I14</f>
+        <v>/servicios</v>
+      </c>
+      <c r="H14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E15" t="str">
+        <f>'End-points'!E15</f>
+        <v>app.post(urlsusers.insertcomentarios,isUser,servicioExist, newComentar)</v>
+      </c>
+      <c r="F15" t="str">
+        <f>'End-points'!I15</f>
+        <v>/users/insert/comentario/:id_ser</v>
+      </c>
+      <c r="H15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E16" t="str">
+        <f>'End-points'!E16</f>
+        <v>app.post(urlsusers.votar,isUser,cannotAdmin, voteServicio)</v>
+      </c>
+      <c r="F16" t="str">
+        <f>'End-points'!I16</f>
+        <v>/servicios/votar/:id_servicio/:id_solucionador</v>
+      </c>
+      <c r="H16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E17" t="str">
+        <f>'End-points'!E17</f>
+        <v>app.post(urls.usersolution,isUser,servicioExist,cannotAdmin,insertSolutions)</v>
+      </c>
+      <c r="F17" t="str">
+        <f>'End-points'!I17</f>
+        <v>/user/solution</v>
+      </c>
+      <c r="H17" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E18" t="str">
+        <f>'End-points'!E18</f>
+        <v>app.get(urlsusers.listarcomentarios,isUser, listComentar)</v>
+      </c>
+      <c r="F18" t="str">
+        <f>'End-points'!I18</f>
+        <v>/comentar</v>
+      </c>
+      <c r="H18" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E19" t="str">
+        <f>'End-points'!E19</f>
+        <v>app.get(urls.users,isUser, listUsers)</v>
+      </c>
+      <c r="F19" t="str">
+        <f>'End-points'!I19</f>
+        <v>/users</v>
+      </c>
+      <c r="H19" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="20" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E20" t="str">
+        <f>'End-points'!E20</f>
+        <v>app.get(urls.servicios,isUser, listServicios);</v>
+      </c>
+      <c r="F20" t="str">
+        <f>'End-points'!I20</f>
+        <v>/servicios</v>
+      </c>
+      <c r="H20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="5:8" x14ac:dyDescent="0.25">
+      <c r="E21" t="str">
+        <f>'End-points'!E21</f>
+        <v xml:space="preserve"> app.post(urls.userlogeado,isUser,adminUser)</v>
+      </c>
+      <c r="F21" t="str">
+        <f>'End-points'!I21</f>
+        <v>/users/userLogin/</v>
+      </c>
+      <c r="H21" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>